<commit_message>
graphs to check classification
at first sight no explanation for the remarkable classifictions
</commit_message>
<xml_diff>
--- a/_PETRO/classificated_counts_higlighted.xlsx
+++ b/_PETRO/classificated_counts_higlighted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_PETRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6521187C-5626-4B56-9D6C-F7923913A8E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D97718-95B9-4CB0-96D6-5A2C7CD1C430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>classificated</t>
   </si>
@@ -94,12 +94,6 @@
     <t>magnesian/calcic/peralkaline</t>
   </si>
   <si>
-    <t>not likely</t>
-  </si>
-  <si>
-    <t>few</t>
-  </si>
-  <si>
     <t>not possible</t>
   </si>
   <si>
@@ -134,6 +128,24 @@
   </si>
   <si>
     <t>alkalic/alkali-calcic</t>
+  </si>
+  <si>
+    <t>still some are pesent</t>
+  </si>
+  <si>
+    <t>feroan calcic seen as one group</t>
+  </si>
+  <si>
+    <t>are metaluminous</t>
+  </si>
+  <si>
+    <t>theoretically possible</t>
+  </si>
+  <si>
+    <t>uncommen</t>
+  </si>
+  <si>
+    <t>Frost, 2011</t>
   </si>
 </sst>
 </file>
@@ -160,7 +172,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +200,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -231,15 +249,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -542,258 +563,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>630</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>605</v>
+        <v>59</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
       </c>
       <c r="O4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>177</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" t="s">
         <v>28</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>492</v>
-      </c>
-      <c r="J5" s="7"/>
-      <c r="K5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>397</v>
+        <v>42</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>397</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" t="s">
         <v>24</v>
       </c>
-      <c r="O6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="O7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="O9" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>346</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>605</v>
+      </c>
+      <c r="O10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q10" t="s">
         <v>36</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>119</v>
+      </c>
+      <c r="O12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>179</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>177</v>
-      </c>
-      <c r="O10" t="s">
-        <v>32</v>
-      </c>
-      <c r="P10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="B16">
-        <v>44</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>17</v>
+      <c r="A18" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>31</v>
+        <v>492</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B19">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="B20">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
+      <c r="A21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>15</v>
+        <v>893</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>21</v>
+      <c r="A22" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>23</v>
+      <c r="A24" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B24">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>